<commit_message>
agregue cositas en la caja diaria y corregi un par de errores
</commit_message>
<xml_diff>
--- a/cajas-diarias/caja-2023-09-07.xlsx
+++ b/cajas-diarias/caja-2023-09-07.xlsx
@@ -397,19 +397,106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>A</v>
+        <v>name</v>
+      </c>
+      <c r="B1" t="str">
+        <v>price</v>
+      </c>
+      <c r="C1" t="str">
+        <v>tipos</v>
+      </c>
+      <c r="D1" t="str">
+        <v>tiposEdad</v>
+      </c>
+      <c r="E1" t="str">
+        <v>tiposMordida</v>
+      </c>
+      <c r="F1" t="str">
+        <v>peso</v>
+      </c>
+      <c r="G1" t="str">
+        <v>option</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>NUTRIBON</v>
+      </c>
+      <c r="B2" t="str">
+        <v>8300</v>
+      </c>
+      <c r="C2" t="str">
+        <v>SUELTO</v>
+      </c>
+      <c r="D2" t="str">
+        <v>ADULTO</v>
+      </c>
+      <c r="E2" t="str">
+        <v>GRANDE</v>
+      </c>
+      <c r="F2" t="str">
+        <v>20</v>
+      </c>
+      <c r="G2" t="str">
+        <v>EFECTIVO</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>NUTRIBON</v>
+      </c>
+      <c r="B3" t="str">
+        <v>4600</v>
+      </c>
+      <c r="C3" t="str">
+        <v>SUELTO</v>
+      </c>
+      <c r="D3" t="str">
+        <v>ADULTO</v>
+      </c>
+      <c r="E3" t="str">
+        <v>PEQUENIA</v>
+      </c>
+      <c r="F3" t="str">
+        <v>8</v>
+      </c>
+      <c r="G3" t="str">
+        <v>EFECTIVO</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>DOGUI</v>
+      </c>
+      <c r="B4" t="str">
+        <v>16000</v>
+      </c>
+      <c r="C4" t="str">
+        <v>PERRO</v>
+      </c>
+      <c r="D4" t="str">
+        <v>ADULTO</v>
+      </c>
+      <c r="E4" t="str">
+        <v>GRANDE</v>
+      </c>
+      <c r="F4" t="str">
+        <v>21</v>
+      </c>
+      <c r="G4" t="str">
+        <v>EFECTIVO</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>